<commit_message>
validator can take single CLI arg specifying Excel file location. JSON file inferred from Excel file path and name. \nsystems.json now contains fully expanded data. Source data in file paths is stored in template_systems.json. \nAll SpaceWire write commands updated for no reply to write command (instruction 0x75). \nCdTe DE now has broadcast readout mode setting command.
</commit_message>
<xml_diff>
--- a/commands/cdte1/cdte1_command_deck.xlsx
+++ b/commands/cdte1/cdte1_command_deck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/commands/cdte1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55E31E5-1BCB-E943-A77C-85DD67A3C2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9459A25F-CF49-2744-8EB2-0C8B6E25F8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -258,9 +258,6 @@
     <t>0x4d</t>
   </si>
   <si>
-    <t>0x7d</t>
-  </si>
-  <si>
     <t>0x3c3c0100000000003c3c3c3c</t>
   </si>
   <si>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t>read MACRO for event data in ring buffer from canister (see Formatter implementation)</t>
+  </si>
+  <si>
+    <t>0x75</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -623,6 +623,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,10 +941,10 @@
   <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD18" sqref="AD18"/>
+      <selection pane="bottomRight" activeCell="Y21" sqref="Y21:Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1370,7 @@
     </row>
     <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>55</v>
@@ -1445,7 +1446,7 @@
         <v>73</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA6" s="25" t="s">
         <v>41</v>
@@ -1454,12 +1455,12 @@
         <v>69</v>
       </c>
       <c r="AC6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>55</v>
@@ -1487,7 +1488,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" s="23" t="s">
         <v>70</v>
@@ -1535,7 +1536,7 @@
         <v>73</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>41</v>
@@ -1544,12 +1545,12 @@
         <v>69</v>
       </c>
       <c r="AC7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>55</v>
@@ -1577,10 +1578,10 @@
         <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -1625,7 +1626,7 @@
         <v>73</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA8" s="25" t="s">
         <v>41</v>
@@ -1634,12 +1635,12 @@
         <v>69</v>
       </c>
       <c r="AC8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>55</v>
@@ -1667,7 +1668,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K9" s="23" t="s">
         <v>70</v>
@@ -1715,7 +1716,7 @@
         <v>73</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA9" s="25" t="s">
         <v>41</v>
@@ -1724,12 +1725,12 @@
         <v>69</v>
       </c>
       <c r="AC9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>55</v>
@@ -1757,10 +1758,10 @@
         <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L10" s="6">
         <v>0</v>
@@ -1805,7 +1806,7 @@
         <v>73</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>41</v>
@@ -1814,12 +1815,12 @@
         <v>69</v>
       </c>
       <c r="AC10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>55</v>
@@ -1847,7 +1848,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K11" s="23" t="s">
         <v>70</v>
@@ -1895,7 +1896,7 @@
         <v>73</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA11" s="25" t="s">
         <v>41</v>
@@ -1904,12 +1905,12 @@
         <v>69</v>
       </c>
       <c r="AC11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>55</v>
@@ -1940,7 +1941,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -1985,7 +1986,7 @@
         <v>73</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA12" s="25" t="s">
         <v>41</v>
@@ -1994,12 +1995,12 @@
         <v>69</v>
       </c>
       <c r="AC12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>55</v>
@@ -2075,7 +2076,7 @@
         <v>73</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA13" s="25" t="s">
         <v>41</v>
@@ -2084,12 +2085,12 @@
         <v>69</v>
       </c>
       <c r="AC13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>55</v>
@@ -2117,7 +2118,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>71</v>
@@ -2165,7 +2166,7 @@
         <v>73</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA14" s="25" t="s">
         <v>41</v>
@@ -2174,12 +2175,12 @@
         <v>69</v>
       </c>
       <c r="AC14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>55</v>
@@ -2210,7 +2211,7 @@
         <v>21</v>
       </c>
       <c r="K15" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L15" s="6">
         <v>0</v>
@@ -2255,7 +2256,7 @@
         <v>73</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>41</v>
@@ -2264,12 +2265,12 @@
         <v>69</v>
       </c>
       <c r="AC15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>55</v>
@@ -2345,7 +2346,7 @@
         <v>73</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA16" s="25" t="s">
         <v>41</v>
@@ -2354,12 +2355,12 @@
         <v>69</v>
       </c>
       <c r="AC16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>55</v>
@@ -2387,7 +2388,7 @@
         <v>17</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K17" s="23" t="s">
         <v>71</v>
@@ -2435,7 +2436,7 @@
         <v>73</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA17" s="25" t="s">
         <v>41</v>
@@ -2444,12 +2445,12 @@
         <v>69</v>
       </c>
       <c r="AC17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>55</v>
@@ -2525,7 +2526,7 @@
         <v>73</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA18" s="25" t="s">
         <v>41</v>
@@ -2534,7 +2535,7 @@
         <v>69</v>
       </c>
       <c r="AC18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2730,7 +2731,7 @@
         <v>68</v>
       </c>
       <c r="Y21" s="22" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="Z21" s="3" t="s">
         <v>41</v>
@@ -2820,7 +2821,7 @@
         <v>68</v>
       </c>
       <c r="Y22" s="22" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="Z22" s="3" t="s">
         <v>41</v>
@@ -2909,8 +2910,8 @@
       <c r="X23" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y23" s="22" t="s">
-        <v>74</v>
+      <c r="Y23" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z23" s="3" t="s">
         <v>41</v>
@@ -2999,8 +3000,8 @@
       <c r="X24" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y24" s="22" t="s">
-        <v>74</v>
+      <c r="Y24" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>41</v>
@@ -3017,7 +3018,7 @@
     </row>
     <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>55</v>
@@ -3089,25 +3090,25 @@
       <c r="X25" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y25" s="22" t="s">
+      <c r="Y25" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA25" s="23" t="s">
         <v>74</v>
-      </c>
-      <c r="Z25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA25" s="23" t="s">
-        <v>75</v>
       </c>
       <c r="AB25" t="s">
         <v>69</v>
       </c>
       <c r="AC25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>55</v>
@@ -3179,25 +3180,25 @@
       <c r="X26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y26" s="22" t="s">
-        <v>74</v>
+      <c r="Y26" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA26" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB26" t="s">
         <v>69</v>
       </c>
       <c r="AC26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>55</v>
@@ -3269,25 +3270,25 @@
       <c r="X27" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y27" s="22" t="s">
-        <v>74</v>
+      <c r="Y27" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA27" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB27" t="s">
         <v>69</v>
       </c>
       <c r="AC27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>55</v>
@@ -3359,25 +3360,25 @@
       <c r="X28" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y28" s="22" t="s">
-        <v>74</v>
+      <c r="Y28" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA28" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB28" t="s">
         <v>69</v>
       </c>
       <c r="AC28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>55</v>
@@ -3449,25 +3450,25 @@
       <c r="X29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y29" s="22" t="s">
-        <v>74</v>
+      <c r="Y29" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA29" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB29" t="s">
         <v>69</v>
       </c>
       <c r="AC29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>55</v>
@@ -3539,25 +3540,25 @@
       <c r="X30" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y30" s="22" t="s">
-        <v>74</v>
+      <c r="Y30" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA30" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AB30" t="s">
         <v>69</v>
       </c>
       <c r="AC30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>55</v>
@@ -3629,25 +3630,25 @@
       <c r="X31" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y31" s="22" t="s">
-        <v>74</v>
+      <c r="Y31" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA31" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB31" t="s">
         <v>69</v>
       </c>
       <c r="AC31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>55</v>
@@ -3659,7 +3660,7 @@
         <v>100001</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>17</v>
@@ -3718,20 +3719,20 @@
       <c r="X32" t="s">
         <v>68</v>
       </c>
-      <c r="Y32" s="3" t="s">
-        <v>74</v>
+      <c r="Y32" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB32" t="s">
         <v>69</v>
       </c>
       <c r="AC32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -3808,8 +3809,8 @@
       <c r="X33" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y33" s="22" t="s">
-        <v>74</v>
+      <c r="Y33" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z33" s="3" t="s">
         <v>41</v>
@@ -3898,8 +3899,8 @@
       <c r="X34" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y34" s="22" t="s">
-        <v>74</v>
+      <c r="Y34" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z34" s="3" t="s">
         <v>41</v>
@@ -3988,8 +3989,8 @@
       <c r="X35" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y35" s="22" t="s">
-        <v>74</v>
+      <c r="Y35" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z35" s="3" t="s">
         <v>41</v>
@@ -4078,8 +4079,8 @@
       <c r="X36" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y36" s="22" t="s">
-        <v>74</v>
+      <c r="Y36" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z36" s="3" t="s">
         <v>41</v>
@@ -4168,8 +4169,8 @@
       <c r="X37" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y37" s="22" t="s">
-        <v>74</v>
+      <c r="Y37" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z37" s="3" t="s">
         <v>41</v>
@@ -4258,8 +4259,8 @@
       <c r="X38" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y38" s="22" t="s">
-        <v>74</v>
+      <c r="Y38" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="Z38" s="3" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
adding order and color fields to all command decks to drive user interface display of commands.
</commit_message>
<xml_diff>
--- a/commands/cdte1/cdte1_command_deck.xlsx
+++ b/commands/cdte1/cdte1_command_deck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cdte1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/GSE/GSE-FOXSI-4/foxsi4-commands/commands/cdte1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09999D6B-1554-154C-82FF-1CFDDEB444AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AB9538-852B-934A-89F3-170D78AD6BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="122">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>0x31c</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>0x000000</t>
+  </si>
+  <si>
+    <t>0xff1741</t>
   </si>
 </sst>
 </file>
@@ -491,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -546,6 +558,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,13 +881,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomRight" activeCell="AE30" sqref="AE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -888,11 +909,13 @@
     <col min="25" max="25" width="12.83203125" style="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.1640625" style="20" customWidth="1"/>
     <col min="27" max="27" width="27.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.1640625" customWidth="1"/>
-    <col min="29" max="29" width="82" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.1640625" customWidth="1"/>
+    <col min="31" max="31" width="82" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
@@ -930,8 +953,10 @@
       </c>
       <c r="Z1" s="28"/>
       <c r="AA1" s="29"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1013,14 +1038,20 @@
       <c r="AA2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>79</v>
       </c>
@@ -1103,14 +1134,20 @@
       <c r="AA3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="32">
+        <v>8</v>
+      </c>
+      <c r="AC3" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD3" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>78</v>
       </c>
@@ -1193,14 +1230,20 @@
       <c r="AA4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AB4" s="32">
+        <v>9</v>
+      </c>
+      <c r="AC4" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD4" t="s">
         <v>39</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>77</v>
       </c>
@@ -1283,14 +1326,20 @@
       <c r="AA5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AB5" s="32">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD5" t="s">
         <v>39</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AE5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>76</v>
       </c>
@@ -1373,14 +1422,20 @@
       <c r="AA6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AB6" s="32">
+        <v>11</v>
+      </c>
+      <c r="AC6" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD6" t="s">
         <v>39</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AE6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>75</v>
       </c>
@@ -1463,14 +1518,20 @@
       <c r="AA7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AB7" s="32">
+        <v>12</v>
+      </c>
+      <c r="AC7" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD7" t="s">
         <v>39</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>74</v>
       </c>
@@ -1553,14 +1614,20 @@
       <c r="AA8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AB8" s="32">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD8" t="s">
         <v>39</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AE8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>80</v>
       </c>
@@ -1643,14 +1710,20 @@
       <c r="AA9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AB9" s="32">
+        <v>14</v>
+      </c>
+      <c r="AC9" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD9" t="s">
         <v>39</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AE9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>81</v>
       </c>
@@ -1733,14 +1806,20 @@
       <c r="AA10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AB10" s="32">
+        <v>15</v>
+      </c>
+      <c r="AC10" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD10" t="s">
         <v>39</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AE10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>82</v>
       </c>
@@ -1823,14 +1902,20 @@
       <c r="AA11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AB11" s="32">
+        <v>16</v>
+      </c>
+      <c r="AC11" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD11" t="s">
         <v>39</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AE11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>83</v>
       </c>
@@ -1913,14 +1998,20 @@
       <c r="AA12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AB12" s="32">
+        <v>17</v>
+      </c>
+      <c r="AC12" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD12" t="s">
         <v>39</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AE12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>84</v>
       </c>
@@ -2003,14 +2094,20 @@
       <c r="AA13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AB13" s="32">
+        <v>18</v>
+      </c>
+      <c r="AC13" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD13" t="s">
         <v>39</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AE13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>85</v>
       </c>
@@ -2093,14 +2190,20 @@
       <c r="AA14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AB14" s="32">
+        <v>19</v>
+      </c>
+      <c r="AC14" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD14" t="s">
         <v>39</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AE14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>111</v>
       </c>
@@ -2183,14 +2286,20 @@
       <c r="AA15" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AB15" s="32">
+        <v>20</v>
+      </c>
+      <c r="AC15" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD15" t="s">
         <v>39</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AE15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>114</v>
       </c>
@@ -2273,14 +2382,20 @@
       <c r="AA16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AB16" s="32">
+        <v>21</v>
+      </c>
+      <c r="AC16" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD16" t="s">
         <v>39</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AE16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -2363,14 +2478,20 @@
       <c r="AA17" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AB17" s="32">
+        <v>22</v>
+      </c>
+      <c r="AC17" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD17" t="s">
         <v>39</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AE17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2397,8 +2518,10 @@
       <c r="Y18" s="24"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="24"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
     </row>
-    <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>50</v>
       </c>
@@ -2481,14 +2604,20 @@
       <c r="AA19" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AB19" s="34">
+        <v>7</v>
+      </c>
+      <c r="AC19" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD19" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AE19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>51</v>
       </c>
@@ -2571,14 +2700,20 @@
       <c r="AA20" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AB20" s="34">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD20" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AE20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>52</v>
       </c>
@@ -2661,14 +2796,20 @@
       <c r="AA21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AB21" s="34">
+        <v>6</v>
+      </c>
+      <c r="AC21" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD21" t="s">
         <v>39</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AE21" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>53</v>
       </c>
@@ -2751,14 +2892,20 @@
       <c r="AA22" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AB22" s="34">
+        <v>2</v>
+      </c>
+      <c r="AC22" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD22" t="s">
         <v>39</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AE22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>54</v>
       </c>
@@ -2841,14 +2988,20 @@
       <c r="AA23" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AB23" s="34">
+        <v>3</v>
+      </c>
+      <c r="AC23" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD23" t="s">
         <v>39</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AE23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>55</v>
       </c>
@@ -2931,14 +3084,20 @@
       <c r="AA24" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AB24" s="34">
+        <v>4</v>
+      </c>
+      <c r="AC24" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD24" t="s">
         <v>39</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AE24" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>56</v>
       </c>
@@ -3021,14 +3180,20 @@
       <c r="AA25" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AB25" s="34">
+        <v>5</v>
+      </c>
+      <c r="AC25" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD25" t="s">
         <v>39</v>
       </c>
-      <c r="AC25" t="s">
+      <c r="AE25" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>102</v>
       </c>
@@ -3110,10 +3275,16 @@
       <c r="AA26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AB26" s="3">
+        <v>23</v>
+      </c>
+      <c r="AC26" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD26" t="s">
         <v>39</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="AE26" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>